<commit_message>
Removed studies 12, 65, 91 which do not have TB mortality
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -1,35 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79BF391-5590-49DF-BC37-93993CEC9926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E172D6-97B6-41EA-B774-738D40367537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
     <sheet name="1029_1055" sheetId="8" r:id="rId2"/>
     <sheet name="1029_1056" sheetId="9" r:id="rId3"/>
     <sheet name="48_1000_1029" sheetId="7" r:id="rId4"/>
-    <sheet name="12" sheetId="19" r:id="rId5"/>
-    <sheet name="44" sheetId="1" r:id="rId6"/>
-    <sheet name="45" sheetId="22" r:id="rId7"/>
-    <sheet name="5_1047" sheetId="14" r:id="rId8"/>
-    <sheet name="63" sheetId="10" r:id="rId9"/>
-    <sheet name="65" sheetId="12" r:id="rId10"/>
-    <sheet name="67" sheetId="23" r:id="rId11"/>
-    <sheet name="75" sheetId="16" r:id="rId12"/>
-    <sheet name="75_1035" sheetId="15" r:id="rId13"/>
-    <sheet name="90_1016" sheetId="17" r:id="rId14"/>
-    <sheet name="91" sheetId="3" r:id="rId15"/>
-    <sheet name="93" sheetId="4" r:id="rId16"/>
-    <sheet name="94" sheetId="5" r:id="rId17"/>
+    <sheet name="44" sheetId="1" r:id="rId5"/>
+    <sheet name="45" sheetId="22" r:id="rId6"/>
+    <sheet name="5_1047" sheetId="14" r:id="rId7"/>
+    <sheet name="63" sheetId="10" r:id="rId8"/>
+    <sheet name="67" sheetId="23" r:id="rId9"/>
+    <sheet name="75" sheetId="16" r:id="rId10"/>
+    <sheet name="75_1035" sheetId="15" r:id="rId11"/>
+    <sheet name="90_1016" sheetId="17" r:id="rId12"/>
+    <sheet name="93" sheetId="4" r:id="rId13"/>
+    <sheet name="94" sheetId="5" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="107">
   <si>
     <t>paper_id</t>
   </si>
@@ -174,24 +171,6 @@
     <t>1029_1056_1</t>
   </si>
   <si>
-    <t>12_1</t>
-  </si>
-  <si>
-    <t>12_2</t>
-  </si>
-  <si>
-    <t>12_3</t>
-  </si>
-  <si>
-    <t>12_4</t>
-  </si>
-  <si>
-    <t>12_5</t>
-  </si>
-  <si>
-    <t>12_6</t>
-  </si>
-  <si>
     <t>44_1</t>
   </si>
   <si>
@@ -249,9 +228,6 @@
     <t>63_15</t>
   </si>
   <si>
-    <t>65_1</t>
-  </si>
-  <si>
     <t>67_1</t>
   </si>
   <si>
@@ -319,42 +295,6 @@
   </si>
   <si>
     <t>90_1016_1</t>
-  </si>
-  <si>
-    <t>91_1</t>
-  </si>
-  <si>
-    <t>91_2</t>
-  </si>
-  <si>
-    <t>91_3</t>
-  </si>
-  <si>
-    <t>91_4</t>
-  </si>
-  <si>
-    <t>91_5</t>
-  </si>
-  <si>
-    <t>91_6</t>
-  </si>
-  <si>
-    <t>91_7</t>
-  </si>
-  <si>
-    <t>91_8</t>
-  </si>
-  <si>
-    <t>91_9</t>
-  </si>
-  <si>
-    <t>91_10</t>
-  </si>
-  <si>
-    <t>91_11</t>
-  </si>
-  <si>
-    <t>91_12</t>
   </si>
   <si>
     <t>93_1</t>
@@ -504,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -523,7 +463,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,7 +917,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>32</v>
@@ -986,10 +925,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -997,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1005,15 +944,15 @@
         <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -1021,15 +960,15 @@
         <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1069,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1077,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1101,7 +1040,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1119,615 +1058,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>65</v>
-      </c>
-      <c r="B2">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>571</v>
-      </c>
-      <c r="L2">
-        <v>310</v>
-      </c>
-      <c r="M2">
-        <v>147</v>
-      </c>
-      <c r="N2">
-        <v>106</v>
-      </c>
-      <c r="P2">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FFEA4-C50F-468E-BF5D-81C19145DAB2}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:Q10"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>67</v>
-      </c>
-      <c r="B2">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="10">
-        <v>334</v>
-      </c>
-      <c r="J2" s="11">
-        <v>5</v>
-      </c>
-      <c r="K2" s="11">
-        <v>2</v>
-      </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10">
-        <v>268</v>
-      </c>
-      <c r="N2" s="10">
-        <v>59</v>
-      </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>67</v>
-      </c>
-      <c r="B3">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3" s="10">
-        <v>326.69461077844312</v>
-      </c>
-      <c r="J3" s="10">
-        <v>3.7634730538922163</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10">
-        <v>245</v>
-      </c>
-      <c r="N3" s="10">
-        <v>28</v>
-      </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10">
-        <v>49.931137724550901</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>67</v>
-      </c>
-      <c r="B4">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4" s="10">
-        <v>272.30210051688113</v>
-      </c>
-      <c r="J4" s="10">
-        <v>4.7915979324755309</v>
-      </c>
-      <c r="K4" s="10">
-        <v>2</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10">
-        <v>138</v>
-      </c>
-      <c r="N4" s="10">
-        <v>17</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10">
-        <v>110.51050258440559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>67</v>
-      </c>
-      <c r="B5">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5" s="10">
-        <v>458</v>
-      </c>
-      <c r="J5" s="10">
-        <v>37</v>
-      </c>
-      <c r="K5" s="10">
-        <v>6</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10">
-        <v>227</v>
-      </c>
-      <c r="N5" s="10">
-        <v>188</v>
-      </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>67</v>
-      </c>
-      <c r="B6">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="10">
-        <v>414.46288209606985</v>
-      </c>
-      <c r="J6" s="10">
-        <v>26.312227074235807</v>
-      </c>
-      <c r="K6" s="10">
-        <v>2</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10">
-        <v>237</v>
-      </c>
-      <c r="N6" s="10">
-        <v>112</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10">
-        <v>37.150655021834062</v>
-      </c>
-      <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>67</v>
-      </c>
-      <c r="B7">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7" s="10">
-        <v>346.56793661496965</v>
-      </c>
-      <c r="J7" s="10">
-        <v>42.240475387727571</v>
-      </c>
-      <c r="K7" s="10">
-        <v>4</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10">
-        <v>152</v>
-      </c>
-      <c r="N7" s="10">
-        <v>43</v>
-      </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10">
-        <v>105.32746122724208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>67</v>
-      </c>
-      <c r="B8">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8" s="10">
-        <v>192</v>
-      </c>
-      <c r="J8" s="10">
-        <v>57</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10">
-        <v>47</v>
-      </c>
-      <c r="N8" s="10">
-        <v>88</v>
-      </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>67</v>
-      </c>
-      <c r="B9">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9" s="10">
-        <v>135</v>
-      </c>
-      <c r="J9" s="10">
-        <v>12.96875</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10">
-        <v>52</v>
-      </c>
-      <c r="N9" s="10">
-        <v>62</v>
-      </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10">
-        <v>7.03125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>67</v>
-      </c>
-      <c r="B10">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10" s="10">
-        <v>113.7037037037037</v>
-      </c>
-      <c r="J10" s="10">
-        <v>31.851851851851848</v>
-      </c>
-      <c r="K10" s="10">
-        <v>1</v>
-      </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10">
-        <v>38</v>
-      </c>
-      <c r="N10" s="10">
-        <v>23</v>
-      </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10">
-        <v>19.851851851851851</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -1750,7 +1080,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1759,13 +1089,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -1806,7 +1136,7 @@
         <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1847,7 +1177,7 @@
         <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1888,7 +1218,7 @@
         <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1929,7 +1259,7 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1970,7 +1300,7 @@
         <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -2011,7 +1341,7 @@
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -2052,7 +1382,7 @@
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -2093,7 +1423,7 @@
         <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -2134,7 +1464,7 @@
         <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -2175,7 +1505,7 @@
         <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -2216,7 +1546,7 @@
         <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -2257,7 +1587,7 @@
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -2298,7 +1628,7 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -2339,7 +1669,7 @@
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
@@ -2380,7 +1710,7 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -2421,7 +1751,7 @@
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -2462,7 +1792,7 @@
         <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -2503,7 +1833,7 @@
         <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -2544,7 +1874,7 @@
         <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -2585,7 +1915,7 @@
         <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -2626,7 +1956,7 @@
         <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -2667,7 +1997,7 @@
         <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
@@ -2708,7 +2038,7 @@
         <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -2749,7 +2079,7 @@
         <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
@@ -2790,7 +2120,7 @@
         <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
@@ -2831,7 +2161,7 @@
         <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2872,7 +2202,7 @@
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
@@ -2913,7 +2243,7 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
@@ -2954,7 +2284,7 @@
         <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -2995,7 +2325,7 @@
         <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
@@ -3062,7 +2392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3085,7 +2415,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3094,13 +2424,13 @@
         <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -3141,10 +2471,10 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -3185,10 +2515,10 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -3229,10 +2559,10 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -3273,10 +2603,10 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -3317,10 +2647,10 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -3361,10 +2691,10 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -3405,10 +2735,10 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -3449,10 +2779,10 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -3493,10 +2823,10 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -3537,10 +2867,10 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -3581,10 +2911,10 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -3625,10 +2955,10 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -3669,10 +2999,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
@@ -3713,10 +3043,10 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -3757,10 +3087,10 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
         <v>24</v>
@@ -3801,10 +3131,10 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -3843,7 +3173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3866,7 +3196,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3875,13 +3205,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -3922,10 +3252,10 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -3960,582 +3290,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:P13"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>91</v>
-      </c>
-      <c r="B2">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14">
-        <v>2.5274999999999999</v>
-      </c>
-      <c r="I2">
-        <v>362</v>
-      </c>
-      <c r="L2">
-        <v>115</v>
-      </c>
-      <c r="M2">
-        <v>92</v>
-      </c>
-      <c r="N2">
-        <v>143</v>
-      </c>
-      <c r="P2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>91</v>
-      </c>
-      <c r="B3">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14">
-        <v>3.6549999999999998</v>
-      </c>
-      <c r="I3">
-        <v>266</v>
-      </c>
-      <c r="L3">
-        <v>91</v>
-      </c>
-      <c r="M3">
-        <v>73</v>
-      </c>
-      <c r="N3">
-        <v>87</v>
-      </c>
-      <c r="P3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>91</v>
-      </c>
-      <c r="B4">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>4.4858333000000004</v>
-      </c>
-      <c r="I4">
-        <v>232</v>
-      </c>
-      <c r="L4">
-        <v>94</v>
-      </c>
-      <c r="M4">
-        <v>72</v>
-      </c>
-      <c r="N4">
-        <v>56</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>91</v>
-      </c>
-      <c r="B5">
-        <v>91</v>
-      </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>5.3108332999999996</v>
-      </c>
-      <c r="I5">
-        <v>239</v>
-      </c>
-      <c r="L5">
-        <v>111</v>
-      </c>
-      <c r="M5">
-        <v>79</v>
-      </c>
-      <c r="N5">
-        <v>39</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>91</v>
-      </c>
-      <c r="B6">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>6.8641667000000002</v>
-      </c>
-      <c r="I6">
-        <v>214</v>
-      </c>
-      <c r="L6">
-        <v>105</v>
-      </c>
-      <c r="M6">
-        <v>57</v>
-      </c>
-      <c r="N6">
-        <v>46</v>
-      </c>
-      <c r="P6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>91</v>
-      </c>
-      <c r="B7">
-        <v>91</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>7.4424999999999999</v>
-      </c>
-      <c r="I7">
-        <v>158</v>
-      </c>
-      <c r="L7">
-        <v>91</v>
-      </c>
-      <c r="M7">
-        <v>44</v>
-      </c>
-      <c r="N7">
-        <v>16</v>
-      </c>
-      <c r="P7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>91</v>
-      </c>
-      <c r="B8">
-        <v>91</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>8.2899999999999991</v>
-      </c>
-      <c r="I8">
-        <v>183</v>
-      </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8">
-        <v>54</v>
-      </c>
-      <c r="N8">
-        <v>18</v>
-      </c>
-      <c r="P8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>91</v>
-      </c>
-      <c r="B9">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14">
-        <v>9.1174999999999997</v>
-      </c>
-      <c r="I9">
-        <v>171</v>
-      </c>
-      <c r="L9">
-        <v>88</v>
-      </c>
-      <c r="M9">
-        <v>44</v>
-      </c>
-      <c r="N9">
-        <v>22</v>
-      </c>
-      <c r="P9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>91</v>
-      </c>
-      <c r="B10">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
-        <v>10.184167</v>
-      </c>
-      <c r="I10">
-        <v>196</v>
-      </c>
-      <c r="L10">
-        <v>106</v>
-      </c>
-      <c r="M10">
-        <v>53</v>
-      </c>
-      <c r="N10">
-        <v>27</v>
-      </c>
-      <c r="P10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>91</v>
-      </c>
-      <c r="B11">
-        <v>91</v>
-      </c>
-      <c r="C11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14">
-        <v>10.9975</v>
-      </c>
-      <c r="I11">
-        <v>231</v>
-      </c>
-      <c r="L11">
-        <v>134</v>
-      </c>
-      <c r="M11">
-        <v>65</v>
-      </c>
-      <c r="N11">
-        <v>24</v>
-      </c>
-      <c r="P11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>91</v>
-      </c>
-      <c r="B12">
-        <v>91</v>
-      </c>
-      <c r="C12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>11.879167000000001</v>
-      </c>
-      <c r="I12">
-        <v>178</v>
-      </c>
-      <c r="L12">
-        <v>89</v>
-      </c>
-      <c r="M12">
-        <v>68</v>
-      </c>
-      <c r="N12">
-        <v>11</v>
-      </c>
-      <c r="P12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>91</v>
-      </c>
-      <c r="B13">
-        <v>91</v>
-      </c>
-      <c r="C13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="14">
-        <v>12.913333</v>
-      </c>
-      <c r="I13">
-        <v>89</v>
-      </c>
-      <c r="L13">
-        <v>33</v>
-      </c>
-      <c r="M13">
-        <v>41</v>
-      </c>
-      <c r="N13">
-        <v>10</v>
-      </c>
-      <c r="P13">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4551,7 +3313,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4560,13 +3322,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -4607,7 +3369,7 @@
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -4648,7 +3410,7 @@
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -4689,7 +3451,7 @@
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -4730,7 +3492,7 @@
         <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4771,7 +3533,7 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -4812,7 +3574,7 @@
         <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -4853,7 +3615,7 @@
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -4894,7 +3656,7 @@
         <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -4935,7 +3697,7 @@
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -4974,15 +3736,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4997,7 +3759,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5006,13 +3768,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -5053,10 +3815,10 @@
         <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -5118,7 +3880,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5127,13 +3889,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -5663,8 +4425,8 @@
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5680,7 +4442,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5689,13 +4451,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -6285,7 +5047,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -6294,13 +5056,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -6341,7 +5103,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -6385,7 +5147,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -6429,7 +5191,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -6473,7 +5235,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -6517,7 +5279,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -6561,7 +5323,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -6605,7 +5367,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -6649,7 +5411,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -6693,7 +5455,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -6737,7 +5499,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -6781,7 +5543,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -6825,7 +5587,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -6869,427 +5631,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:P9"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1.5</v>
-      </c>
-      <c r="I2">
-        <v>126</v>
-      </c>
-      <c r="L2">
-        <v>38</v>
-      </c>
-      <c r="M2">
-        <v>35</v>
-      </c>
-      <c r="N2">
-        <v>53</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>1.5</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>88</v>
-      </c>
-      <c r="L3">
-        <v>13</v>
-      </c>
-      <c r="M3">
-        <v>44</v>
-      </c>
-      <c r="N3">
-        <v>31</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3">
-        <v>5</v>
-      </c>
-      <c r="I4" s="3">
-        <v>75</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
-        <v>11</v>
-      </c>
-      <c r="M4" s="3">
-        <v>41</v>
-      </c>
-      <c r="N4" s="3">
-        <v>23</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="3">
-        <v>154</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3">
-        <v>38</v>
-      </c>
-      <c r="M5" s="3">
-        <v>50</v>
-      </c>
-      <c r="N5" s="3">
-        <v>66</v>
-      </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>136</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3">
-        <v>23</v>
-      </c>
-      <c r="M6" s="3">
-        <v>53</v>
-      </c>
-      <c r="N6" s="3">
-        <v>60</v>
-      </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>119</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3">
-        <v>28</v>
-      </c>
-      <c r="M7" s="3">
-        <v>29</v>
-      </c>
-      <c r="N7" s="3">
-        <v>62</v>
-      </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>70</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3">
-        <v>9</v>
-      </c>
-      <c r="M8" s="3">
-        <v>33</v>
-      </c>
-      <c r="N8" s="3">
-        <v>21</v>
-      </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3">
-        <v>40</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3">
-        <v>15</v>
-      </c>
-      <c r="M9" s="3">
-        <v>11</v>
-      </c>
-      <c r="N9" s="3">
-        <v>13</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7312,7 +5653,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -7321,13 +5662,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -7368,10 +5709,10 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -7410,10 +5751,10 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -7452,10 +5793,10 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -7494,10 +5835,10 @@
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -7536,10 +5877,10 @@
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -7578,10 +5919,10 @@
         <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -7620,10 +5961,10 @@
         <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -7662,10 +6003,10 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -7704,10 +6045,10 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -7746,10 +6087,10 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -7788,10 +6129,10 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -7828,7 +6169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545D6599-22A2-41A6-A0C4-4AA22E18DB81}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7852,7 +6193,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -7861,13 +6202,13 @@
         <v>38</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>36</v>
@@ -7908,7 +6249,7 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>12</v>
@@ -7954,7 +6295,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
@@ -8000,7 +6341,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -8046,7 +6387,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -8092,7 +6433,7 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -8137,7 +6478,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -8182,7 +6523,7 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -8227,7 +6568,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -8272,7 +6613,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>12</v>
@@ -8317,7 +6658,7 @@
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
@@ -8362,7 +6703,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>12</v>
@@ -8407,7 +6748,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -8452,7 +6793,7 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -8496,7 +6837,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>12</v>
@@ -8540,7 +6881,7 @@
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -8585,7 +6926,7 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
@@ -8629,7 +6970,7 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
@@ -8673,7 +7014,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>12</v>
@@ -8717,7 +7058,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -8761,7 +7102,7 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>12</v>
@@ -8805,7 +7146,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>13</v>
@@ -8849,7 +7190,7 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>13</v>
@@ -8893,7 +7234,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>13</v>
@@ -8937,7 +7278,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
@@ -8981,7 +7322,7 @@
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>13</v>
@@ -9025,7 +7366,7 @@
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>13</v>
@@ -9069,7 +7410,7 @@
         <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>13</v>
@@ -9113,7 +7454,7 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
@@ -9157,7 +7498,7 @@
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>13</v>
@@ -9201,7 +7542,7 @@
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>13</v>
@@ -9245,7 +7586,7 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>13</v>
@@ -9289,7 +7630,7 @@
         <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>13</v>
@@ -9333,7 +7674,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>13</v>
@@ -9377,7 +7718,7 @@
         <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>13</v>
@@ -9421,7 +7762,7 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>13</v>
@@ -9465,7 +7806,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>13</v>
@@ -9509,7 +7850,7 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>13</v>
@@ -9553,7 +7894,7 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>13</v>
@@ -9597,7 +7938,7 @@
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>13</v>
@@ -9641,7 +7982,7 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>13</v>
@@ -9703,7 +8044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9727,7 +8068,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -9736,13 +8077,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -9783,10 +8124,10 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
@@ -9824,10 +8165,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>18</v>
@@ -9866,7 +8207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9889,7 +8230,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -9898,13 +8239,13 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>36</v>
@@ -9945,10 +8286,10 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -9986,10 +8327,10 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -10027,10 +8368,10 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -10068,10 +8409,10 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -10109,10 +8450,10 @@
         <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -10150,7 +8491,7 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -10191,7 +8532,7 @@
         <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -10232,7 +8573,7 @@
         <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -10273,7 +8614,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -10314,7 +8655,7 @@
         <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -10355,7 +8696,7 @@
         <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -10396,7 +8737,7 @@
         <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -10437,7 +8778,7 @@
         <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -10478,7 +8819,7 @@
         <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -10519,7 +8860,7 @@
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -10550,6 +8891,498 @@
       </c>
       <c r="P16">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FFEA4-C50F-468E-BF5D-81C19145DAB2}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="10">
+        <v>334</v>
+      </c>
+      <c r="J2" s="11">
+        <v>5</v>
+      </c>
+      <c r="K2" s="11">
+        <v>2</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10">
+        <v>268</v>
+      </c>
+      <c r="N2" s="10">
+        <v>59</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="10">
+        <v>326.69461077844312</v>
+      </c>
+      <c r="J3" s="10">
+        <v>3.7634730538922163</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10">
+        <v>245</v>
+      </c>
+      <c r="N3" s="10">
+        <v>28</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10">
+        <v>49.931137724550901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="10">
+        <v>272.30210051688113</v>
+      </c>
+      <c r="J4" s="10">
+        <v>4.7915979324755309</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10">
+        <v>138</v>
+      </c>
+      <c r="N4" s="10">
+        <v>17</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10">
+        <v>110.51050258440559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="10">
+        <v>458</v>
+      </c>
+      <c r="J5" s="10">
+        <v>37</v>
+      </c>
+      <c r="K5" s="10">
+        <v>6</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10">
+        <v>227</v>
+      </c>
+      <c r="N5" s="10">
+        <v>188</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="10">
+        <v>414.46288209606985</v>
+      </c>
+      <c r="J6" s="10">
+        <v>26.312227074235807</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10">
+        <v>237</v>
+      </c>
+      <c r="N6" s="10">
+        <v>112</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10">
+        <v>37.150655021834062</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>67</v>
+      </c>
+      <c r="B7">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" s="10">
+        <v>346.56793661496965</v>
+      </c>
+      <c r="J7" s="10">
+        <v>42.240475387727571</v>
+      </c>
+      <c r="K7" s="10">
+        <v>4</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10">
+        <v>152</v>
+      </c>
+      <c r="N7" s="10">
+        <v>43</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10">
+        <v>105.32746122724208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="10">
+        <v>192</v>
+      </c>
+      <c r="J8" s="10">
+        <v>57</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10">
+        <v>47</v>
+      </c>
+      <c r="N8" s="10">
+        <v>88</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" s="10">
+        <v>135</v>
+      </c>
+      <c r="J9" s="10">
+        <v>12.96875</v>
+      </c>
+      <c r="K9" s="10">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10">
+        <v>52</v>
+      </c>
+      <c r="N9" s="10">
+        <v>62</v>
+      </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10">
+        <v>7.03125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="10">
+        <v>113.7037037037037</v>
+      </c>
+      <c r="J10" s="10">
+        <v>31.851851851851848</v>
+      </c>
+      <c r="K10" s="10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10">
+        <v>38</v>
+      </c>
+      <c r="N10" s="10">
+        <v>23</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10">
+        <v>19.851851851851851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed all-cause mortality analysis
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E172D6-97B6-41EA-B774-738D40367537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B79C52-0942-4DDD-818C-26BE44C2685F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3298,7 +3298,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removed all-cause mortality figures
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B79C52-0942-4DDD-818C-26BE44C2685F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ADE027-2C6D-413E-9484-C67C6028A181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="90_1016" sheetId="17" r:id="rId12"/>
     <sheet name="93" sheetId="4" r:id="rId13"/>
     <sheet name="94" sheetId="5" r:id="rId14"/>
+    <sheet name="79_1023" sheetId="24" r:id="rId15"/>
+    <sheet name="79_1023_sev" sheetId="25" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="115">
   <si>
     <t>paper_id</t>
   </si>
@@ -370,6 +372,30 @@
   </si>
   <si>
     <t>N alive (sum of self-cured and chronic; only included if study does not provide cure data)</t>
+  </si>
+  <si>
+    <t>79_1023</t>
+  </si>
+  <si>
+    <t>79_1023_1</t>
+  </si>
+  <si>
+    <t>79_1023_2</t>
+  </si>
+  <si>
+    <t>79_1023_3</t>
+  </si>
+  <si>
+    <t>79_1023_4</t>
+  </si>
+  <si>
+    <t>79_1023_5</t>
+  </si>
+  <si>
+    <t>79_1023_6</t>
+  </si>
+  <si>
+    <t>79_1023_7</t>
   </si>
 </sst>
 </file>
@@ -903,10 +929,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,9 +1088,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2394,9 +2420,6 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3175,9 +3198,6 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3292,13 +3312,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3738,13 +3755,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3856,11 +3870,1245 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB2BA5-051F-4879-AA33-720BFC715E78}">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>607</v>
+      </c>
+      <c r="J2">
+        <v>226</v>
+      </c>
+      <c r="P2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>351</v>
+      </c>
+      <c r="J3">
+        <v>105</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>236</v>
+      </c>
+      <c r="J4">
+        <v>49</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>186</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>150</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>130</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>119</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>112</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>99</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>96</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>89</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>85</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>82</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>77</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>397</v>
+      </c>
+      <c r="J16">
+        <v>119</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>275</v>
+      </c>
+      <c r="J17">
+        <v>55</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>217</v>
+      </c>
+      <c r="J18">
+        <v>28</v>
+      </c>
+      <c r="P18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>183</v>
+      </c>
+      <c r="J19">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>153</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>131</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>119</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>273</v>
+      </c>
+      <c r="J23">
+        <v>72</v>
+      </c>
+      <c r="P23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>192</v>
+      </c>
+      <c r="J24">
+        <v>29</v>
+      </c>
+      <c r="P24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>157</v>
+      </c>
+      <c r="J25">
+        <v>23</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>133</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>114</v>
+      </c>
+      <c r="J27">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>241</v>
+      </c>
+      <c r="J28">
+        <v>67</v>
+      </c>
+      <c r="P28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>162</v>
+      </c>
+      <c r="J29">
+        <v>32</v>
+      </c>
+      <c r="P29">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B28F9FC-CBCB-4ADB-875E-BC9399F2D87A}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>155</v>
+      </c>
+      <c r="J3">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>63</v>
+      </c>
+      <c r="N3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>587</v>
+      </c>
+      <c r="J4">
+        <v>354</v>
+      </c>
+      <c r="M4">
+        <v>98</v>
+      </c>
+      <c r="N4">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4420,9 +5668,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
@@ -5025,13 +6270,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5632,13 +6874,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6171,13 +7410,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545D6599-22A2-41A6-A0C4-4AA22E18DB81}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8046,9 +9282,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8209,13 +9442,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8901,9 +10131,6 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FFEA4-C50F-468E-BF5D-81C19145DAB2}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Reran analysis with new papers and no all-cause mortality
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75114E-4998-4EB9-80E9-ACD5B43A4A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F804E484-4D65-43C5-8303-A179E08E91B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3874,13 +3874,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB2BA5-051F-4879-AA33-720BFC715E78}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3947,10 +3949,10 @@
         <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3963,6 +3965,9 @@
       </c>
       <c r="J2">
         <v>226</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
       <c r="P2">
         <v>30</v>
@@ -3982,10 +3987,10 @@
         <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3998,6 +4003,9 @@
       </c>
       <c r="J3">
         <v>105</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -4017,10 +4025,10 @@
         <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -4033,6 +4041,9 @@
       </c>
       <c r="J4">
         <v>49</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -4052,10 +4063,10 @@
         <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -4068,6 +4079,9 @@
       </c>
       <c r="J5">
         <v>31</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
       </c>
       <c r="P5">
         <v>5</v>
@@ -4087,10 +4101,10 @@
         <v>103</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -4103,6 +4117,9 @@
       </c>
       <c r="J6">
         <v>18</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
       <c r="P6">
         <v>2</v>
@@ -4122,10 +4139,10 @@
         <v>103</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -4138,6 +4155,9 @@
       </c>
       <c r="J7">
         <v>11</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -4157,10 +4177,10 @@
         <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -4173,6 +4193,9 @@
       </c>
       <c r="J8">
         <v>5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="P8">
         <v>2</v>
@@ -4192,10 +4215,10 @@
         <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>7</v>
@@ -4208,6 +4231,9 @@
       </c>
       <c r="J9">
         <v>11</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="P9">
         <v>2</v>
@@ -4227,10 +4253,10 @@
         <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -4243,6 +4269,9 @@
       </c>
       <c r="J10">
         <v>3</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -4262,10 +4291,10 @@
         <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -4278,6 +4307,9 @@
       </c>
       <c r="J11">
         <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -4297,10 +4329,10 @@
         <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -4313,6 +4345,9 @@
       </c>
       <c r="J12">
         <v>3</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -4332,10 +4367,10 @@
         <v>103</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>11</v>
@@ -4348,6 +4383,9 @@
       </c>
       <c r="J13">
         <v>3</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -4367,10 +4405,10 @@
         <v>103</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>12</v>
@@ -4383,6 +4421,9 @@
       </c>
       <c r="J14">
         <v>4</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -4402,10 +4443,10 @@
         <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G15">
         <v>13</v>
@@ -4418,6 +4459,9 @@
       </c>
       <c r="J15">
         <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -4437,10 +4481,10 @@
         <v>103</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -4453,6 +4497,9 @@
       </c>
       <c r="J16">
         <v>119</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
       <c r="P16">
         <v>3</v>
@@ -4472,10 +4519,10 @@
         <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -4488,6 +4535,9 @@
       </c>
       <c r="J17">
         <v>55</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
       <c r="P17">
         <v>3</v>
@@ -4507,10 +4557,10 @@
         <v>103</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -4523,6 +4573,9 @@
       </c>
       <c r="J18">
         <v>28</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
       <c r="P18">
         <v>6</v>
@@ -4542,10 +4595,10 @@
         <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -4558,6 +4611,9 @@
       </c>
       <c r="J19">
         <v>25</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
       </c>
       <c r="P19">
         <v>5</v>
@@ -4577,10 +4633,10 @@
         <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -4593,6 +4649,9 @@
       </c>
       <c r="J20">
         <v>20</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
       </c>
       <c r="P20">
         <v>2</v>
@@ -4612,10 +4671,10 @@
         <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -4628,6 +4687,9 @@
       </c>
       <c r="J21">
         <v>12</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -4647,10 +4709,10 @@
         <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G22">
         <v>6</v>
@@ -4663,6 +4725,9 @@
       </c>
       <c r="J22">
         <v>7</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -4682,10 +4747,10 @@
         <v>103</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -4698,6 +4763,9 @@
       </c>
       <c r="J23">
         <v>72</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
       </c>
       <c r="P23">
         <v>9</v>
@@ -4717,10 +4785,10 @@
         <v>103</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -4733,6 +4801,9 @@
       </c>
       <c r="J24">
         <v>29</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
       </c>
       <c r="P24">
         <v>6</v>
@@ -4752,10 +4823,10 @@
         <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -4768,6 +4839,9 @@
       </c>
       <c r="J25">
         <v>23</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -4787,10 +4861,10 @@
         <v>103</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G26">
         <v>3</v>
@@ -4803,6 +4877,9 @@
       </c>
       <c r="J26">
         <v>18</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -4822,10 +4899,10 @@
         <v>103</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G27">
         <v>4</v>
@@ -4838,6 +4915,9 @@
       </c>
       <c r="J27">
         <v>10</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
       </c>
       <c r="P27">
         <v>0</v>
@@ -4857,10 +4937,10 @@
         <v>103</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -4873,6 +4953,9 @@
       </c>
       <c r="J28">
         <v>67</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
       </c>
       <c r="P28">
         <v>12</v>
@@ -4892,10 +4975,10 @@
         <v>103</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -4908,6 +4991,9 @@
       </c>
       <c r="J29">
         <v>32</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
       </c>
       <c r="P29">
         <v>3</v>
@@ -4924,15 +5010,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B28F9FC-CBCB-4ADB-875E-BC9399F2D87A}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
@@ -5002,10 +5088,10 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -5019,11 +5105,17 @@
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
       <c r="M2">
         <v>3</v>
       </c>
       <c r="N2">
         <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -5040,10 +5132,10 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -5057,11 +5149,17 @@
       <c r="J3">
         <v>46</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
       <c r="M3">
         <v>63</v>
       </c>
       <c r="N3">
         <v>46</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -5078,10 +5176,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5095,11 +5193,17 @@
       <c r="J4">
         <v>354</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="M4">
         <v>98</v>
       </c>
       <c r="N4">
         <v>135</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data from foreign language papers
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\TB Projects\Duration Research\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F804E484-4D65-43C5-8303-A179E08E91B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="2" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
@@ -29,8 +28,12 @@
     <sheet name="94" sheetId="5" r:id="rId14"/>
     <sheet name="79_1023" sheetId="24" r:id="rId15"/>
     <sheet name="79_1023_sev" sheetId="25" r:id="rId16"/>
+    <sheet name="75_1019" sheetId="26" r:id="rId17"/>
+    <sheet name="75_1020" sheetId="27" r:id="rId18"/>
+    <sheet name="75_1021" sheetId="28" r:id="rId19"/>
+    <sheet name="79_1054" sheetId="29" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="138">
   <si>
     <t>paper_id</t>
   </si>
@@ -397,11 +400,80 @@
   <si>
     <t>79_1023_7</t>
   </si>
+  <si>
+    <t>75_1019</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>75_1020</t>
+  </si>
+  <si>
+    <t>79_1021</t>
+  </si>
+  <si>
+    <t>79_1021_1</t>
+  </si>
+  <si>
+    <t>79_1021_2</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>79_1021_3</t>
+  </si>
+  <si>
+    <t>79_1021_4</t>
+  </si>
+  <si>
+    <t>79_1021_5</t>
+  </si>
+  <si>
+    <t>79_1021_6</t>
+  </si>
+  <si>
+    <t>79_1021_7</t>
+  </si>
+  <si>
+    <t>79_1021_8</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>79_1054</t>
+  </si>
+  <si>
+    <t>79_1054_1</t>
+  </si>
+  <si>
+    <t>79_1054_2</t>
+  </si>
+  <si>
+    <t>79_1054_3</t>
+  </si>
+  <si>
+    <t>79_1054_4</t>
+  </si>
+  <si>
+    <t>79_1054_5</t>
+  </si>
+  <si>
+    <t>79_1054_6</t>
+  </si>
+  <si>
+    <t>79_1054_7</t>
+  </si>
+  <si>
+    <t>79_1054_8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -928,14 +1000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2419,11 +2491,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3197,7 +3269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3311,7 +3383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3754,7 +3826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3871,11 +3943,11 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB2BA5-051F-4879-AA33-720BFC715E78}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5007,7 +5079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B28F9FC-CBCB-4ADB-875E-BC9399F2D87A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5211,8 +5283,1478 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="20.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>2022</v>
+      </c>
+      <c r="L2">
+        <v>1094</v>
+      </c>
+      <c r="M2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>1949</v>
+      </c>
+      <c r="L3">
+        <v>1178</v>
+      </c>
+      <c r="M3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>1872</v>
+      </c>
+      <c r="L4">
+        <v>1240</v>
+      </c>
+      <c r="M4">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>1804</v>
+      </c>
+      <c r="L5">
+        <v>1285</v>
+      </c>
+      <c r="M5">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>1731</v>
+      </c>
+      <c r="L6">
+        <v>1314</v>
+      </c>
+      <c r="M6">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>1658</v>
+      </c>
+      <c r="L7">
+        <v>1336</v>
+      </c>
+      <c r="M7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>1627</v>
+      </c>
+      <c r="L8">
+        <v>1355</v>
+      </c>
+      <c r="M8">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>670</v>
+      </c>
+      <c r="L2">
+        <v>32</v>
+      </c>
+      <c r="M2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>541</v>
+      </c>
+      <c r="L3">
+        <v>99</v>
+      </c>
+      <c r="M3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>477</v>
+      </c>
+      <c r="L4">
+        <v>130</v>
+      </c>
+      <c r="M4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>448</v>
+      </c>
+      <c r="L5">
+        <v>148</v>
+      </c>
+      <c r="M5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>397</v>
+      </c>
+      <c r="L6">
+        <v>160</v>
+      </c>
+      <c r="M6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>357</v>
+      </c>
+      <c r="L7">
+        <v>164</v>
+      </c>
+      <c r="M7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>311</v>
+      </c>
+      <c r="L8">
+        <v>174</v>
+      </c>
+      <c r="M8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>277</v>
+      </c>
+      <c r="L9">
+        <v>179</v>
+      </c>
+      <c r="M9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>243</v>
+      </c>
+      <c r="L10">
+        <v>181</v>
+      </c>
+      <c r="M10">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>280</v>
+      </c>
+      <c r="M2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>280</v>
+      </c>
+      <c r="M3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>280</v>
+      </c>
+      <c r="M4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>280</v>
+      </c>
+      <c r="M5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>280</v>
+      </c>
+      <c r="M6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>259</v>
+      </c>
+      <c r="M7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>259</v>
+      </c>
+      <c r="M8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>259</v>
+      </c>
+      <c r="M9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>345</v>
+      </c>
+      <c r="M10">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>345</v>
+      </c>
+      <c r="M11">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>247</v>
+      </c>
+      <c r="M12">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>985</v>
+      </c>
+      <c r="M13">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>985</v>
+      </c>
+      <c r="M14">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>985</v>
+      </c>
+      <c r="M15">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>985</v>
+      </c>
+      <c r="M16">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>985</v>
+      </c>
+      <c r="M17">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>849</v>
+      </c>
+      <c r="M18">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>849</v>
+      </c>
+      <c r="M19">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>849</v>
+      </c>
+      <c r="M20">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>479</v>
+      </c>
+      <c r="M21">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>479</v>
+      </c>
+      <c r="M22">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>171</v>
+      </c>
+      <c r="M23">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5770,11 +7312,311 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>637</v>
+      </c>
+      <c r="M2">
+        <v>268</v>
+      </c>
+      <c r="P2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>1189</v>
+      </c>
+      <c r="M3">
+        <v>541</v>
+      </c>
+      <c r="P3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>1308</v>
+      </c>
+      <c r="M4">
+        <v>523</v>
+      </c>
+      <c r="P4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1195</v>
+      </c>
+      <c r="M5">
+        <v>484</v>
+      </c>
+      <c r="P5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>747</v>
+      </c>
+      <c r="M6">
+        <v>377</v>
+      </c>
+      <c r="P6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1603</v>
+      </c>
+      <c r="M7">
+        <v>818</v>
+      </c>
+      <c r="P7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>1309</v>
+      </c>
+      <c r="M8">
+        <v>637</v>
+      </c>
+      <c r="P8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1150</v>
+      </c>
+      <c r="M9">
+        <v>555</v>
+      </c>
+      <c r="P9">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -6373,7 +8215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
@@ -6977,7 +8819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
@@ -7513,7 +9355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545D6599-22A2-41A6-A0C4-4AA22E18DB81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
@@ -9385,7 +11227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -9545,10 +11387,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -10234,7 +12076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FFEA4-C50F-468E-BF5D-81C19145DAB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Added foreign language cure data
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="138">
   <si>
     <t>paper_id</t>
   </si>
@@ -7317,7 +7317,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7388,6 +7388,12 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
       <c r="G2">
         <v>0</v>
       </c>
@@ -7417,6 +7423,12 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
       <c r="G3">
         <v>0</v>
       </c>
@@ -7446,6 +7458,12 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
       <c r="G4">
         <v>0</v>
       </c>
@@ -7475,6 +7493,12 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
       <c r="G5">
         <v>0</v>
       </c>
@@ -7504,6 +7528,12 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -7533,6 +7563,12 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -7562,6 +7598,12 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
       <c r="G8">
         <v>0</v>
       </c>
@@ -7590,6 +7632,12 @@
       </c>
       <c r="D9" t="s">
         <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
       </c>
       <c r="G9">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed issue with new study
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\TB Projects\Duration Research\pre_chemo_tb\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FB64AE-2720-4FDC-B171-AE538A7542A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" firstSheet="4" activeTab="19"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
@@ -33,7 +34,7 @@
     <sheet name="75_1021" sheetId="28" r:id="rId19"/>
     <sheet name="79_1054" sheetId="29" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,6 +45,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -470,7 +472,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -997,7 +999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1156,7 +1158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2488,7 +2490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3266,7 +3268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3380,7 +3382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3823,7 +3825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3940,7 +3942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5076,7 +5078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5281,11 +5283,11 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5595,7 +5597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5979,10 +5981,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -6751,10 +6753,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -7310,11 +7312,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7658,7 +7660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8260,7 +8262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
@@ -8864,7 +8866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
@@ -9400,7 +9402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -11272,7 +11274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -11432,7 +11434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -12121,7 +12123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
fixed error on alling papers
</commit_message>
<xml_diff>
--- a/data/pre_chemo_data.xlsx
+++ b/data/pre_chemo_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Boston University\Duration_of_Infectiousness\pre_chemo_tb\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfwhite\Documents\GitHub\pre_chemo_tb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E06C97-19A2-41F6-AF36-FE3A9E9496BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-108" windowWidth="19176" windowHeight="6924" tabRatio="866" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data dictionary" sheetId="2" r:id="rId1"/>
@@ -538,7 +537,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1066,7 +1065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1225,7 +1224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798C8DE4-7802-4B27-BB1D-E5088A3F512A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1331,7 +1330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1820,7 +1819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3152,7 +3151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3930,7 +3929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4044,10 +4043,10 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D901BE-BDC0-4DF6-8001-FF237FE8D52F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -4601,7 +4600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5044,7 +5043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5161,7 +5160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6297,7 +6296,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6502,10 +6501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7061,7 +7060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7377,7 +7376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7763,7 +7762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8535,7 +8534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8883,7 +8882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -9485,11 +9484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10089,7 +10088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BDEA05-FBAA-4009-9E6B-33104F16EEF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10499,7 +10498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
@@ -11035,7 +11034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12907,7 +12906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -13067,7 +13066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">

</xml_diff>